<commit_message>
data update - gform responses
</commit_message>
<xml_diff>
--- a/google_sheet_data.xlsx
+++ b/google_sheet_data.xlsx
@@ -4555,7 +4555,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>12LPA</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -4577,7 +4577,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>12LPA</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -10759,7 +10759,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
@@ -10781,7 +10781,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C471" t="inlineStr">
@@ -10803,7 +10803,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
@@ -10825,7 +10825,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
@@ -10847,7 +10847,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
@@ -10869,7 +10869,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C475" t="inlineStr">
@@ -10891,7 +10891,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C476" t="inlineStr">
@@ -10913,7 +10913,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C477" t="inlineStr">
@@ -10935,7 +10935,7 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
@@ -10957,7 +10957,7 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.29LPA</t>
         </is>
       </c>
       <c r="C479" t="inlineStr">
@@ -10979,7 +10979,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.29LPA</t>
         </is>
       </c>
       <c r="C480" t="inlineStr">
@@ -11001,7 +11001,7 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.29LPA</t>
         </is>
       </c>
       <c r="C481" t="inlineStr">
@@ -11221,7 +11221,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>13.5LPA</t>
+          <t>16.84LPA</t>
         </is>
       </c>
       <c r="C491" t="inlineStr">

</xml_diff>

<commit_message>
dup hpe r&d ctc up
</commit_message>
<xml_diff>
--- a/google_sheet_data.xlsx
+++ b/google_sheet_data.xlsx
@@ -71402,7 +71402,7 @@
       </c>
       <c r="B2629" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>17.5LPA</t>
         </is>
       </c>
       <c r="C2629" t="inlineStr">
@@ -71429,7 +71429,7 @@
       </c>
       <c r="B2630" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>17.5LPA</t>
         </is>
       </c>
       <c r="C2630" t="inlineStr">
@@ -71456,7 +71456,7 @@
       </c>
       <c r="B2631" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>17.5LPA</t>
         </is>
       </c>
       <c r="C2631" t="inlineStr">
@@ -71483,7 +71483,7 @@
       </c>
       <c r="B2632" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>17.5LPA</t>
         </is>
       </c>
       <c r="C2632" t="inlineStr">
@@ -71510,7 +71510,7 @@
       </c>
       <c r="B2633" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>17.5LPA</t>
         </is>
       </c>
       <c r="C2633" t="inlineStr">
@@ -71537,7 +71537,7 @@
       </c>
       <c r="B2634" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>17.5LPA</t>
         </is>
       </c>
       <c r="C2634" t="inlineStr">
@@ -71564,7 +71564,7 @@
       </c>
       <c r="B2635" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>17.5LPA</t>
         </is>
       </c>
       <c r="C2635" t="inlineStr">
@@ -71591,7 +71591,7 @@
       </c>
       <c r="B2636" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>17.5LPA</t>
         </is>
       </c>
       <c r="C2636" t="inlineStr">

</xml_diff>

<commit_message>
bbt add and dup
</commit_message>
<xml_diff>
--- a/google_sheet_data.xlsx
+++ b/google_sheet_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3251"/>
+  <dimension ref="A1:E3252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -88215,6 +88215,33 @@
         </is>
       </c>
     </row>
+    <row r="3252">
+      <c r="A3252" t="inlineStr">
+        <is>
+          <t>21BRS1147</t>
+        </is>
+      </c>
+      <c r="B3252" t="inlineStr">
+        <is>
+          <t>7.5LPA</t>
+        </is>
+      </c>
+      <c r="C3252" t="inlineStr">
+        <is>
+          <t>Volvo</t>
+        </is>
+      </c>
+      <c r="D3252" t="inlineStr">
+        <is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="E3252" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
dup and updates expander
</commit_message>
<xml_diff>
--- a/google_sheet_data.xlsx
+++ b/google_sheet_data.xlsx
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>27.8LPA</t>
+          <t>43.2LPA</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>27.8LPA</t>
+          <t>43.2LPA</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>27.8LPA</t>
+          <t>43.2LPA</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>27.8LPA</t>
+          <t>43.2LPA</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>27.8LPA</t>
+          <t>43.2LPA</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>27.8LPA</t>
+          <t>43.2LPA</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1791,7 +1791,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>27.8LPA</t>
+          <t>43.2LPA</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">

</xml_diff>

<commit_message>
option to combine witch and normal offers and NA
</commit_message>
<xml_diff>
--- a/google_sheet_data.xlsx
+++ b/google_sheet_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3330"/>
+  <dimension ref="A1:E3339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -657,7 +657,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>33LPA</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>33LPA</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33LPA</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -738,7 +738,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>33LPA</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -765,7 +765,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>33LPA</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -69323,7 +69323,7 @@
       </c>
       <c r="B2552" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2552" t="inlineStr">
@@ -69350,7 +69350,7 @@
       </c>
       <c r="B2553" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2553" t="inlineStr">
@@ -69377,7 +69377,7 @@
       </c>
       <c r="B2554" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2554" t="inlineStr">
@@ -69404,7 +69404,7 @@
       </c>
       <c r="B2555" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2555" t="inlineStr">
@@ -69431,7 +69431,7 @@
       </c>
       <c r="B2556" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2556" t="inlineStr">
@@ -69458,7 +69458,7 @@
       </c>
       <c r="B2557" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2557" t="inlineStr">
@@ -69485,7 +69485,7 @@
       </c>
       <c r="B2558" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2558" t="inlineStr">
@@ -69512,7 +69512,7 @@
       </c>
       <c r="B2559" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2559" t="inlineStr">
@@ -69539,7 +69539,7 @@
       </c>
       <c r="B2560" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2560" t="inlineStr">
@@ -69566,7 +69566,7 @@
       </c>
       <c r="B2561" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2561" t="inlineStr">
@@ -69593,7 +69593,7 @@
       </c>
       <c r="B2562" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2562" t="inlineStr">
@@ -69620,7 +69620,7 @@
       </c>
       <c r="B2563" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2563" t="inlineStr">
@@ -69647,7 +69647,7 @@
       </c>
       <c r="B2564" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2564" t="inlineStr">
@@ -69674,7 +69674,7 @@
       </c>
       <c r="B2565" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2565" t="inlineStr">
@@ -69701,7 +69701,7 @@
       </c>
       <c r="B2566" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2566" t="inlineStr">
@@ -69728,7 +69728,7 @@
       </c>
       <c r="B2567" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2567" t="inlineStr">
@@ -69755,7 +69755,7 @@
       </c>
       <c r="B2568" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2568" t="inlineStr">
@@ -69782,7 +69782,7 @@
       </c>
       <c r="B2569" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2569" t="inlineStr">
@@ -69809,7 +69809,7 @@
       </c>
       <c r="B2570" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2570" t="inlineStr">
@@ -69836,7 +69836,7 @@
       </c>
       <c r="B2571" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2571" t="inlineStr">
@@ -69863,7 +69863,7 @@
       </c>
       <c r="B2572" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2572" t="inlineStr">
@@ -69890,7 +69890,7 @@
       </c>
       <c r="B2573" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2573" t="inlineStr">
@@ -69917,7 +69917,7 @@
       </c>
       <c r="B2574" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2574" t="inlineStr">
@@ -69944,7 +69944,7 @@
       </c>
       <c r="B2575" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2575" t="inlineStr">
@@ -69971,7 +69971,7 @@
       </c>
       <c r="B2576" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2576" t="inlineStr">
@@ -69998,7 +69998,7 @@
       </c>
       <c r="B2577" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2577" t="inlineStr">
@@ -70025,7 +70025,7 @@
       </c>
       <c r="B2578" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2578" t="inlineStr">
@@ -70052,7 +70052,7 @@
       </c>
       <c r="B2579" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2579" t="inlineStr">
@@ -70079,7 +70079,7 @@
       </c>
       <c r="B2580" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>16.5LPA</t>
         </is>
       </c>
       <c r="C2580" t="inlineStr">
@@ -90343,6 +90343,249 @@
         </is>
       </c>
       <c r="E3330" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3331">
+      <c r="A3331" t="inlineStr">
+        <is>
+          <t>21BLC1531</t>
+        </is>
+      </c>
+      <c r="B3331" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3331" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="D3331" t="inlineStr">
+        <is>
+          <t>BLC</t>
+        </is>
+      </c>
+      <c r="E3331" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3332">
+      <c r="A3332" t="inlineStr">
+        <is>
+          <t>21BCE2959</t>
+        </is>
+      </c>
+      <c r="B3332" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3332" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="D3332" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3332" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3333">
+      <c r="A3333" t="inlineStr">
+        <is>
+          <t>21BIT0179</t>
+        </is>
+      </c>
+      <c r="B3333" t="inlineStr">
+        <is>
+          <t>29LPA</t>
+        </is>
+      </c>
+      <c r="C3333" t="inlineStr">
+        <is>
+          <t>NVIDIA</t>
+        </is>
+      </c>
+      <c r="D3333" t="inlineStr">
+        <is>
+          <t>BIT</t>
+        </is>
+      </c>
+      <c r="E3333" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3334">
+      <c r="A3334" t="inlineStr">
+        <is>
+          <t>21BCE1910</t>
+        </is>
+      </c>
+      <c r="B3334" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3334" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="D3334" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3334" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3335">
+      <c r="A3335" t="inlineStr">
+        <is>
+          <t>21BRS1342</t>
+        </is>
+      </c>
+      <c r="B3335" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3335" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="D3335" t="inlineStr">
+        <is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="E3335" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3336">
+      <c r="A3336" t="inlineStr">
+        <is>
+          <t>21BCE5986</t>
+        </is>
+      </c>
+      <c r="B3336" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3336" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="D3336" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3336" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3337">
+      <c r="A3337" t="inlineStr">
+        <is>
+          <t>21BCE5024</t>
+        </is>
+      </c>
+      <c r="B3337" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3337" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="D3337" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3337" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3338">
+      <c r="A3338" t="inlineStr">
+        <is>
+          <t>21BEC1365</t>
+        </is>
+      </c>
+      <c r="B3338" t="inlineStr">
+        <is>
+          <t>5.25LPA</t>
+        </is>
+      </c>
+      <c r="C3338" t="inlineStr">
+        <is>
+          <t>Renault Nissan</t>
+        </is>
+      </c>
+      <c r="D3338" t="inlineStr">
+        <is>
+          <t>BEC</t>
+        </is>
+      </c>
+      <c r="E3338" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3339">
+      <c r="A3339" t="inlineStr">
+        <is>
+          <t>21BEC2163</t>
+        </is>
+      </c>
+      <c r="B3339" t="inlineStr">
+        <is>
+          <t>9LPA</t>
+        </is>
+      </c>
+      <c r="C3339" t="inlineStr">
+        <is>
+          <t>Lumenci</t>
+        </is>
+      </c>
+      <c r="D3339" t="inlineStr">
+        <is>
+          <t>BEC</t>
+        </is>
+      </c>
+      <c r="E3339" t="inlineStr">
         <is>
           <t>Male</t>
         </is>

</xml_diff>

<commit_message>
dup and latest selctions
</commit_message>
<xml_diff>
--- a/google_sheet_data.xlsx
+++ b/google_sheet_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3351"/>
+  <dimension ref="A1:E3380"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -90915,6 +90915,789 @@
         </is>
       </c>
     </row>
+    <row r="3352">
+      <c r="A3352" t="inlineStr">
+        <is>
+          <t>21BCE5141</t>
+        </is>
+      </c>
+      <c r="B3352" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3352" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="D3352" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3352" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3353">
+      <c r="A3353" t="inlineStr">
+        <is>
+          <t>21BCE10295</t>
+        </is>
+      </c>
+      <c r="B3353" t="inlineStr">
+        <is>
+          <t>12LPA</t>
+        </is>
+      </c>
+      <c r="C3353" t="inlineStr">
+        <is>
+          <t>Cimpress</t>
+        </is>
+      </c>
+      <c r="D3353" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3353" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3354">
+      <c r="A3354" t="inlineStr">
+        <is>
+          <t>21BME0261</t>
+        </is>
+      </c>
+      <c r="B3354" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3354" t="inlineStr">
+        <is>
+          <t>Proscape</t>
+        </is>
+      </c>
+      <c r="D3354" t="inlineStr">
+        <is>
+          <t>BME</t>
+        </is>
+      </c>
+      <c r="E3354" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3355">
+      <c r="A3355" t="inlineStr">
+        <is>
+          <t>21BCE2345</t>
+        </is>
+      </c>
+      <c r="B3355" t="inlineStr">
+        <is>
+          <t>7.6LPA</t>
+        </is>
+      </c>
+      <c r="C3355" t="inlineStr">
+        <is>
+          <t>EY Global Delivery Services</t>
+        </is>
+      </c>
+      <c r="D3355" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3355" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3356">
+      <c r="A3356" t="inlineStr">
+        <is>
+          <t>21BCE5705</t>
+        </is>
+      </c>
+      <c r="B3356" t="inlineStr">
+        <is>
+          <t>7.6LPA</t>
+        </is>
+      </c>
+      <c r="C3356" t="inlineStr">
+        <is>
+          <t>EY Global Delivery Services</t>
+        </is>
+      </c>
+      <c r="D3356" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3356" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3357">
+      <c r="A3357" t="inlineStr">
+        <is>
+          <t>21BAI10157</t>
+        </is>
+      </c>
+      <c r="B3357" t="inlineStr">
+        <is>
+          <t>7.6LPA</t>
+        </is>
+      </c>
+      <c r="C3357" t="inlineStr">
+        <is>
+          <t>EY Global Delivery Services</t>
+        </is>
+      </c>
+      <c r="D3357" t="inlineStr">
+        <is>
+          <t>BAI</t>
+        </is>
+      </c>
+      <c r="E3357" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3358">
+      <c r="A3358" t="inlineStr">
+        <is>
+          <t>21BCE7864</t>
+        </is>
+      </c>
+      <c r="B3358" t="inlineStr">
+        <is>
+          <t>7.6LPA</t>
+        </is>
+      </c>
+      <c r="C3358" t="inlineStr">
+        <is>
+          <t>EY Global Delivery Services</t>
+        </is>
+      </c>
+      <c r="D3358" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3358" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3359">
+      <c r="A3359" t="inlineStr">
+        <is>
+          <t>21BCE0611</t>
+        </is>
+      </c>
+      <c r="B3359" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3359" t="inlineStr">
+        <is>
+          <t>BALKAN ID</t>
+        </is>
+      </c>
+      <c r="D3359" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3359" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3360">
+      <c r="A3360" t="inlineStr">
+        <is>
+          <t>21BLC1562</t>
+        </is>
+      </c>
+      <c r="B3360" t="inlineStr">
+        <is>
+          <t>24LPA</t>
+        </is>
+      </c>
+      <c r="C3360" t="inlineStr">
+        <is>
+          <t>Wells Fargo</t>
+        </is>
+      </c>
+      <c r="D3360" t="inlineStr">
+        <is>
+          <t>BLC</t>
+        </is>
+      </c>
+      <c r="E3360" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3361">
+      <c r="A3361" t="inlineStr">
+        <is>
+          <t>21BCE1406</t>
+        </is>
+      </c>
+      <c r="B3361" t="inlineStr">
+        <is>
+          <t>24LPA</t>
+        </is>
+      </c>
+      <c r="C3361" t="inlineStr">
+        <is>
+          <t>Wells Fargo</t>
+        </is>
+      </c>
+      <c r="D3361" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3361" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3362">
+      <c r="A3362" t="inlineStr">
+        <is>
+          <t>21BCE2091</t>
+        </is>
+      </c>
+      <c r="B3362" t="inlineStr">
+        <is>
+          <t>24LPA</t>
+        </is>
+      </c>
+      <c r="C3362" t="inlineStr">
+        <is>
+          <t>Wells Fargo</t>
+        </is>
+      </c>
+      <c r="D3362" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3362" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3363">
+      <c r="A3363" t="inlineStr">
+        <is>
+          <t>21BCE2957</t>
+        </is>
+      </c>
+      <c r="B3363" t="inlineStr">
+        <is>
+          <t>24LPA</t>
+        </is>
+      </c>
+      <c r="C3363" t="inlineStr">
+        <is>
+          <t>Wells Fargo</t>
+        </is>
+      </c>
+      <c r="D3363" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3363" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3364">
+      <c r="A3364" t="inlineStr">
+        <is>
+          <t>21BIT0319</t>
+        </is>
+      </c>
+      <c r="B3364" t="inlineStr">
+        <is>
+          <t>24LPA</t>
+        </is>
+      </c>
+      <c r="C3364" t="inlineStr">
+        <is>
+          <t>Wells Fargo</t>
+        </is>
+      </c>
+      <c r="D3364" t="inlineStr">
+        <is>
+          <t>BIT</t>
+        </is>
+      </c>
+      <c r="E3364" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3365">
+      <c r="A3365" t="inlineStr">
+        <is>
+          <t>21BRS1595</t>
+        </is>
+      </c>
+      <c r="B3365" t="inlineStr">
+        <is>
+          <t>24LPA</t>
+        </is>
+      </c>
+      <c r="C3365" t="inlineStr">
+        <is>
+          <t>Wells Fargo</t>
+        </is>
+      </c>
+      <c r="D3365" t="inlineStr">
+        <is>
+          <t>BRS</t>
+        </is>
+      </c>
+      <c r="E3365" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3366">
+      <c r="A3366" t="inlineStr">
+        <is>
+          <t>21BBS0115</t>
+        </is>
+      </c>
+      <c r="B3366" t="inlineStr">
+        <is>
+          <t>24LPA</t>
+        </is>
+      </c>
+      <c r="C3366" t="inlineStr">
+        <is>
+          <t>Wells Fargo</t>
+        </is>
+      </c>
+      <c r="D3366" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="E3366" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3367">
+      <c r="A3367" t="inlineStr">
+        <is>
+          <t>21BKT0107</t>
+        </is>
+      </c>
+      <c r="B3367" t="inlineStr">
+        <is>
+          <t>24LPA</t>
+        </is>
+      </c>
+      <c r="C3367" t="inlineStr">
+        <is>
+          <t>Wells Fargo</t>
+        </is>
+      </c>
+      <c r="D3367" t="inlineStr">
+        <is>
+          <t>BKT</t>
+        </is>
+      </c>
+      <c r="E3367" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3368">
+      <c r="A3368" t="inlineStr">
+        <is>
+          <t>21BCE1314</t>
+        </is>
+      </c>
+      <c r="B3368" t="inlineStr">
+        <is>
+          <t>24LPA</t>
+        </is>
+      </c>
+      <c r="C3368" t="inlineStr">
+        <is>
+          <t>Wells Fargo</t>
+        </is>
+      </c>
+      <c r="D3368" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3368" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3369">
+      <c r="A3369" t="inlineStr">
+        <is>
+          <t>21BCI0264</t>
+        </is>
+      </c>
+      <c r="B3369" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3369" t="inlineStr">
+        <is>
+          <t>Walmart</t>
+        </is>
+      </c>
+      <c r="D3369" t="inlineStr">
+        <is>
+          <t>BCI</t>
+        </is>
+      </c>
+      <c r="E3369" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3370">
+      <c r="A3370" t="inlineStr">
+        <is>
+          <t>21BCI0042</t>
+        </is>
+      </c>
+      <c r="B3370" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3370" t="inlineStr">
+        <is>
+          <t>Walmart</t>
+        </is>
+      </c>
+      <c r="D3370" t="inlineStr">
+        <is>
+          <t>BCI</t>
+        </is>
+      </c>
+      <c r="E3370" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3371">
+      <c r="A3371" t="inlineStr">
+        <is>
+          <t>21BCI0335</t>
+        </is>
+      </c>
+      <c r="B3371" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3371" t="inlineStr">
+        <is>
+          <t>Walmart</t>
+        </is>
+      </c>
+      <c r="D3371" t="inlineStr">
+        <is>
+          <t>BCI</t>
+        </is>
+      </c>
+      <c r="E3371" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3372">
+      <c r="A3372" t="inlineStr">
+        <is>
+          <t>21BCI0158</t>
+        </is>
+      </c>
+      <c r="B3372" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3372" t="inlineStr">
+        <is>
+          <t>Walmart</t>
+        </is>
+      </c>
+      <c r="D3372" t="inlineStr">
+        <is>
+          <t>BCI</t>
+        </is>
+      </c>
+      <c r="E3372" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3373">
+      <c r="A3373" t="inlineStr">
+        <is>
+          <t>21BCI0055</t>
+        </is>
+      </c>
+      <c r="B3373" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3373" t="inlineStr">
+        <is>
+          <t>Walmart</t>
+        </is>
+      </c>
+      <c r="D3373" t="inlineStr">
+        <is>
+          <t>BCI</t>
+        </is>
+      </c>
+      <c r="E3373" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3374">
+      <c r="A3374" t="inlineStr">
+        <is>
+          <t>21BCI0101</t>
+        </is>
+      </c>
+      <c r="B3374" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3374" t="inlineStr">
+        <is>
+          <t>Walmart</t>
+        </is>
+      </c>
+      <c r="D3374" t="inlineStr">
+        <is>
+          <t>BCI</t>
+        </is>
+      </c>
+      <c r="E3374" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3375">
+      <c r="A3375" t="inlineStr">
+        <is>
+          <t>21BCI0152</t>
+        </is>
+      </c>
+      <c r="B3375" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C3375" t="inlineStr">
+        <is>
+          <t>Walmart</t>
+        </is>
+      </c>
+      <c r="D3375" t="inlineStr">
+        <is>
+          <t>BCI</t>
+        </is>
+      </c>
+      <c r="E3375" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3376">
+      <c r="A3376" t="inlineStr">
+        <is>
+          <t>21BAI1439</t>
+        </is>
+      </c>
+      <c r="B3376" t="inlineStr">
+        <is>
+          <t>8LPA</t>
+        </is>
+      </c>
+      <c r="C3376" t="inlineStr">
+        <is>
+          <t>RELX Group (Elsevier)</t>
+        </is>
+      </c>
+      <c r="D3376" t="inlineStr">
+        <is>
+          <t>BAI</t>
+        </is>
+      </c>
+      <c r="E3376" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3377">
+      <c r="A3377" t="inlineStr">
+        <is>
+          <t>21BCE10047</t>
+        </is>
+      </c>
+      <c r="B3377" t="inlineStr">
+        <is>
+          <t>8LPA</t>
+        </is>
+      </c>
+      <c r="C3377" t="inlineStr">
+        <is>
+          <t>RELX Group (Elsevier)</t>
+        </is>
+      </c>
+      <c r="D3377" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="E3377" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
+    <row r="3378">
+      <c r="A3378" t="inlineStr">
+        <is>
+          <t>21BBS0257</t>
+        </is>
+      </c>
+      <c r="B3378" t="inlineStr">
+        <is>
+          <t>18LPA</t>
+        </is>
+      </c>
+      <c r="C3378" t="inlineStr">
+        <is>
+          <t>Blackrock</t>
+        </is>
+      </c>
+      <c r="D3378" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="E3378" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3379">
+      <c r="A3379" t="inlineStr">
+        <is>
+          <t>21BDS0002</t>
+        </is>
+      </c>
+      <c r="B3379" t="inlineStr">
+        <is>
+          <t>14.5LPA</t>
+        </is>
+      </c>
+      <c r="C3379" t="inlineStr">
+        <is>
+          <t>Philips</t>
+        </is>
+      </c>
+      <c r="D3379" t="inlineStr">
+        <is>
+          <t>BDS</t>
+        </is>
+      </c>
+      <c r="E3379" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
+    <row r="3380">
+      <c r="A3380" t="inlineStr">
+        <is>
+          <t>21BME0075</t>
+        </is>
+      </c>
+      <c r="B3380" t="inlineStr">
+        <is>
+          <t>8.5LPA</t>
+        </is>
+      </c>
+      <c r="C3380" t="inlineStr">
+        <is>
+          <t>Whirlpool</t>
+        </is>
+      </c>
+      <c r="D3380" t="inlineStr">
+        <is>
+          <t>BME</t>
+        </is>
+      </c>
+      <c r="E3380" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>